<commit_message>
added carcass excel gen
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/recap/carcass.xlsx
+++ b/CustomLabelPrinter/recap/carcass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\recap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5FEE44-3BBE-418B-A978-36467E7941AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D596A42E-E72C-4340-B3DD-DC51ACFC4A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14955" yWindow="2370" windowWidth="22935" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="1095" windowWidth="22935" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CARCASS" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +111,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -381,60 +392,84 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,8 +755,8 @@
   </sheetPr>
   <dimension ref="B1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="50" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -732,54 +767,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
     </row>
     <row r="2" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="2:16" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -812,17 +847,17 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="25"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="36">
+      <c r="C5" s="33">
         <v>22486</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -833,13 +868,13 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="31"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="47"/>
     </row>
     <row r="6" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -850,13 +885,13 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="33"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="49"/>
     </row>
     <row r="7" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -867,13 +902,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="33"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="37"/>
     </row>
     <row r="8" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -884,13 +919,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="33"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="37"/>
     </row>
     <row r="9" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -901,13 +936,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="33"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="37"/>
     </row>
     <row r="10" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -918,13 +953,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="33"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="37"/>
     </row>
     <row r="11" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -935,13 +970,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="33"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="37"/>
     </row>
     <row r="12" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -952,13 +987,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="33"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="37"/>
     </row>
     <row r="13" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -969,13 +1004,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="33"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="37"/>
     </row>
     <row r="14" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -986,13 +1021,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="33"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="37"/>
     </row>
     <row r="15" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -1005,13 +1040,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="33"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="37"/>
     </row>
     <row r="16" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -1022,30 +1057,30 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="33"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="37"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="15"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="33"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="37"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -1056,13 +1091,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="33"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="37"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1073,13 +1108,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="33"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="37"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -1090,13 +1125,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="33"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="37"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="27"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1107,13 +1142,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="33"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="37"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1124,13 +1159,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="33"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="37"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="27"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -1141,13 +1176,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="33"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="37"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -1158,13 +1193,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="33"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="37"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="27"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -1175,13 +1210,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="33"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="37"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="27"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -1192,13 +1227,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="33"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="37"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1209,13 +1244,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="35"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="39"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="37"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1226,13 +1261,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="31"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="41"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -1243,13 +1278,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="33"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="43"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -1260,13 +1295,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="33"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="43"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="27"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -1277,13 +1312,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="33"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="43"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -1294,13 +1329,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="33"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="43"/>
     </row>
     <row r="33" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -1311,13 +1346,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="33"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="43"/>
     </row>
     <row r="34" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="27"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -1328,13 +1363,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="33"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="43"/>
     </row>
     <row r="35" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -1345,13 +1380,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="33"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="43"/>
     </row>
     <row r="36" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="27"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -1362,13 +1397,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="33"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="43"/>
     </row>
     <row r="37" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="27"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -1379,13 +1414,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="33"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="43"/>
     </row>
     <row r="38" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="32"/>
       <c r="E38" s="4"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1396,13 +1431,13 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="13"/>
-      <c r="O38" s="34"/>
-      <c r="P38" s="35"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="45"/>
     </row>
     <row r="39" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="15"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="6"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -1413,13 +1448,13 @@
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
       <c r="N39" s="10"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="31"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="41"/>
     </row>
     <row r="40" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="15"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="27"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="11"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -1430,13 +1465,13 @@
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="12"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="33"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="43"/>
     </row>
     <row r="41" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="15"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="27"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -1447,13 +1482,13 @@
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="12"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="33"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="43"/>
     </row>
     <row r="42" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="15"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="27"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="30"/>
       <c r="E42" s="11"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -1464,13 +1499,13 @@
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="N42" s="12"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="33"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="43"/>
     </row>
     <row r="43" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="15"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="27"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
       <c r="E43" s="11"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -1481,13 +1516,13 @@
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="12"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="33"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="43"/>
     </row>
     <row r="44" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="15"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="27"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="11"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -1498,13 +1533,13 @@
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="12"/>
-      <c r="O44" s="32"/>
-      <c r="P44" s="33"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="43"/>
     </row>
     <row r="45" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="15"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="27"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="11"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -1515,12 +1550,12 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="12"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="33"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="43"/>
     </row>
     <row r="46" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="26"/>
-      <c r="D46" s="27"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="11"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
@@ -1531,12 +1566,12 @@
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="12"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="33"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="43"/>
     </row>
     <row r="47" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="26"/>
-      <c r="D47" s="27"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="11"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -1547,12 +1582,12 @@
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="12"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="33"/>
+      <c r="O47" s="42"/>
+      <c r="P47" s="43"/>
     </row>
     <row r="48" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="26"/>
-      <c r="D48" s="27"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="11"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
@@ -1563,12 +1598,12 @@
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="12"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="33"/>
+      <c r="O48" s="42"/>
+      <c r="P48" s="43"/>
     </row>
     <row r="49" spans="3:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="28"/>
-      <c r="D49" s="29"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -1579,11 +1614,11 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="13"/>
-      <c r="O49" s="34"/>
-      <c r="P49" s="35"/>
+      <c r="O49" s="44"/>
+      <c r="P49" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="C28:D29"/>
     <mergeCell ref="C30:D38"/>
     <mergeCell ref="C41:D49"/>
@@ -1595,9 +1630,10 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="C7:D27"/>
-    <mergeCell ref="O5:P27"/>
     <mergeCell ref="C5:D6"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="O7:P27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added breast Gen and tender Gen
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/recap/carcass.xlsx
+++ b/CustomLabelPrinter/recap/carcass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\recap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D596A42E-E72C-4340-B3DD-DC51ACFC4A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FA85EE-0864-47E9-AE57-39DB0431F12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="1095" windowWidth="22935" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22410" yWindow="1095" windowWidth="23385" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CARCASS" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,12 +116,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -395,6 +389,42 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -407,24 +437,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,34 +452,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,54 +761,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
     </row>
     <row r="4" spans="2:16" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -847,17 +841,17 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="28"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="33">
+      <c r="C5" s="25">
         <v>22486</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -873,8 +867,8 @@
     </row>
     <row r="6" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -890,8 +884,8 @@
     </row>
     <row r="7" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -902,13 +896,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="37"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="43"/>
     </row>
     <row r="8" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -919,13 +913,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="37"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="43"/>
     </row>
     <row r="9" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -936,13 +930,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="37"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="43"/>
     </row>
     <row r="10" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -953,13 +947,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="37"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="43"/>
     </row>
     <row r="11" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -970,13 +964,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="37"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="43"/>
     </row>
     <row r="12" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -987,13 +981,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="37"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="43"/>
     </row>
     <row r="13" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -1004,13 +998,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="37"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="43"/>
     </row>
     <row r="14" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -1021,13 +1015,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="37"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="43"/>
     </row>
     <row r="15" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -1040,13 +1034,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="37"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="43"/>
     </row>
     <row r="16" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="30"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -1057,13 +1051,13 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="37"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="43"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="15"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
@@ -1074,13 +1068,13 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="37"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="43"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -1091,13 +1085,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="37"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="43"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1108,13 +1102,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="37"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="43"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -1125,13 +1119,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="37"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="43"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1142,13 +1136,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="37"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="43"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="30"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1159,13 +1153,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="37"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="43"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -1176,13 +1170,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="37"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="43"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -1193,13 +1187,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="37"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="43"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -1210,13 +1204,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="37"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="43"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -1227,13 +1221,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="37"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="43"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1244,13 +1238,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="39"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="45"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="34"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1261,13 +1255,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="41"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="32"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -1278,13 +1272,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="43"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="34"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -1295,13 +1289,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="43"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="34"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -1312,13 +1306,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="43"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="34"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -1329,13 +1323,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="43"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="34"/>
     </row>
     <row r="33" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -1346,13 +1340,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="43"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="34"/>
     </row>
     <row r="34" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -1363,13 +1357,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="43"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="34"/>
     </row>
     <row r="35" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -1380,13 +1374,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="43"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="34"/>
     </row>
     <row r="36" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="28"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -1397,13 +1391,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="43"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="34"/>
     </row>
     <row r="37" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -1414,13 +1408,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="43"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="34"/>
     </row>
     <row r="38" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="32"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
       <c r="E38" s="4"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1431,13 +1425,13 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="13"/>
-      <c r="O38" s="44"/>
-      <c r="P38" s="45"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="36"/>
     </row>
     <row r="39" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="15"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="34"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="26"/>
       <c r="E39" s="6"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -1448,13 +1442,13 @@
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
       <c r="N39" s="10"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="41"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="32"/>
     </row>
     <row r="40" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="15"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="28"/>
       <c r="E40" s="11"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -1465,13 +1459,13 @@
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="12"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="43"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="34"/>
     </row>
     <row r="41" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="15"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28"/>
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -1482,13 +1476,13 @@
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="12"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="43"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="34"/>
     </row>
     <row r="42" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="15"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="30"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="28"/>
       <c r="E42" s="11"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -1499,13 +1493,13 @@
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="N42" s="12"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="43"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="34"/>
     </row>
     <row r="43" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="15"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="30"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
       <c r="E43" s="11"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -1516,13 +1510,13 @@
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="12"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="43"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="34"/>
     </row>
     <row r="44" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="15"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="30"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="28"/>
       <c r="E44" s="11"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -1533,13 +1527,13 @@
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="12"/>
-      <c r="O44" s="42"/>
-      <c r="P44" s="43"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="34"/>
     </row>
     <row r="45" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="15"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="30"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28"/>
       <c r="E45" s="11"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -1550,12 +1544,12 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="12"/>
-      <c r="O45" s="42"/>
-      <c r="P45" s="43"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="34"/>
     </row>
     <row r="46" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="29"/>
-      <c r="D46" s="30"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="28"/>
       <c r="E46" s="11"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
@@ -1566,12 +1560,12 @@
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="12"/>
-      <c r="O46" s="42"/>
-      <c r="P46" s="43"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="34"/>
     </row>
     <row r="47" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="29"/>
-      <c r="D47" s="30"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
       <c r="E47" s="11"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -1582,12 +1576,12 @@
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="12"/>
-      <c r="O47" s="42"/>
-      <c r="P47" s="43"/>
+      <c r="O47" s="33"/>
+      <c r="P47" s="34"/>
     </row>
     <row r="48" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="29"/>
-      <c r="D48" s="30"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="28"/>
       <c r="E48" s="11"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
@@ -1598,12 +1592,12 @@
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="12"/>
-      <c r="O48" s="42"/>
-      <c r="P48" s="43"/>
+      <c r="O48" s="33"/>
+      <c r="P48" s="34"/>
     </row>
     <row r="49" spans="3:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="31"/>
-      <c r="D49" s="32"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -1614,17 +1608,11 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="13"/>
-      <c r="O49" s="44"/>
-      <c r="P49" s="45"/>
+      <c r="O49" s="35"/>
+      <c r="P49" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="C30:D38"/>
-    <mergeCell ref="C41:D49"/>
-    <mergeCell ref="O39:P49"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="O28:P38"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="F2:K3"/>
     <mergeCell ref="N2:O2"/>
@@ -1634,6 +1622,12 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="O5:P6"/>
     <mergeCell ref="O7:P27"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="C30:D38"/>
+    <mergeCell ref="C41:D49"/>
+    <mergeCell ref="O39:P49"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="O28:P38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>

</xml_diff>